<commit_message>
added all sectors and filtered data. Sector comparisons done
</commit_message>
<xml_diff>
--- a/data/sector_correlations/total_intra.xlsx
+++ b/data/sector_correlations/total_intra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deliar/Downloads/courses/CPSC572/672_final/data/sector_correlations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D6301-881A-904D-BC88-4DB9A6EEC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189D604D-11FF-924F-AE08-D204599996EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="176">
   <si>
     <t>Sector</t>
   </si>
@@ -34,31 +34,67 @@
     <t>Min Correlation</t>
   </si>
   <si>
-    <t>Energy Equipment &amp; Services</t>
+    <t>Multi-Utilities(19)</t>
+  </si>
+  <si>
+    <t>(0.9085339576171104, 'CMS', 'WEC')</t>
+  </si>
+  <si>
+    <t>(-0.022110581485324188, 'AEF', 'ED')</t>
+  </si>
+  <si>
+    <t>Industrial Conglomerates(6)</t>
+  </si>
+  <si>
+    <t>(0.7423969814905563, 'HON', 'ROP')</t>
+  </si>
+  <si>
+    <t>(0, 'stock', 'stock')</t>
+  </si>
+  <si>
+    <t>Energy Equipment &amp; Services(34)</t>
   </si>
   <si>
     <t>(0.8882941728141304, 'HAL', 'SLB')</t>
   </si>
   <si>
-    <t>(0, 'stock', 'stock')</t>
-  </si>
-  <si>
-    <t>Airlines</t>
+    <t>Construction Materials(8)</t>
+  </si>
+  <si>
+    <t>(0.8092591332032857, 'MLM', 'VMC')</t>
+  </si>
+  <si>
+    <t>Road &amp; Rail(23)</t>
+  </si>
+  <si>
+    <t>(0.829895696574278, 'CSX', 'NSC')</t>
+  </si>
+  <si>
+    <t>(-0.11459971471402075, 'ARCB', 'DSM')</t>
+  </si>
+  <si>
+    <t>Airlines(15)</t>
   </si>
   <si>
     <t>(0.8928999467636979, 'CEA', 'ZNH')</t>
   </si>
   <si>
-    <t>Equity Real Estate Investment Trusts ...</t>
-  </si>
-  <si>
-    <t>(0.9126866521624862, 'KIM', 'REG')</t>
-  </si>
-  <si>
-    <t>(-0.12823799536807146, 'IHT', 'SBAC')</t>
-  </si>
-  <si>
-    <t>Electric Utilities</t>
+    <t>Auto Components(21)</t>
+  </si>
+  <si>
+    <t>(0.7883215563934879, 'BWA', 'DAN')</t>
+  </si>
+  <si>
+    <t>Blank Check / SPAC(32)</t>
+  </si>
+  <si>
+    <t>(0.8298173193964029, 'AOD', 'GDV')</t>
+  </si>
+  <si>
+    <t>(-0.03627371446698335, 'GSS', 'RCG')</t>
+  </si>
+  <si>
+    <t>Electric Utilities(29)</t>
   </si>
   <si>
     <t>(0.8963693868337042, 'LNT', 'XEL')</t>
@@ -67,7 +103,13 @@
     <t>(-0.1286715503196716, 'EDN', 'MGF')</t>
   </si>
   <si>
-    <t>Hotels, Restaurants &amp; Leisure</t>
+    <t>Containers &amp; Packaging(14)</t>
+  </si>
+  <si>
+    <t>(0.73334832175076, 'IP', 'PKG')</t>
+  </si>
+  <si>
+    <t>Hotels, Restaurants &amp; Leisure(54)</t>
   </si>
   <si>
     <t>(0.9866427501699437, 'CCL', 'CUK')</t>
@@ -76,7 +118,7 @@
     <t>(-0.06058279447573067, 'CPHC', 'TAST')</t>
   </si>
   <si>
-    <t>Machinery</t>
+    <t>Machinery(93)</t>
   </si>
   <si>
     <t>(0.8504897147877548, 'VKI', 'VKQ')</t>
@@ -85,7 +127,22 @@
     <t>(-0.2018622560312524, 'HURC', 'VKQ')</t>
   </si>
   <si>
-    <t>Banks</t>
+    <t>Building Products(27)</t>
+  </si>
+  <si>
+    <t>(0.7005375149402394, 'LII', 'MAS')</t>
+  </si>
+  <si>
+    <t>(-0.13487518218866845, 'APT', 'JEQ')</t>
+  </si>
+  <si>
+    <t>Air Freight &amp; Logistics(12)</t>
+  </si>
+  <si>
+    <t>(0.7089809973042577, 'FDX', 'UPS')</t>
+  </si>
+  <si>
+    <t>Banks(271)</t>
   </si>
   <si>
     <t>(0.9390549555893505, 'BBD', 'ITUB')</t>
@@ -94,7 +151,13 @@
     <t>(-0.25630984505676646, 'EGF', 'MCBC')</t>
   </si>
   <si>
-    <t>Trading Companies &amp; Distributors</t>
+    <t>Multiline Retail(8)</t>
+  </si>
+  <si>
+    <t>(0.7288556457235531, 'KSS', 'M')</t>
+  </si>
+  <si>
+    <t>Trading Companies &amp; Distributors(28)</t>
   </si>
   <si>
     <t>(0.7824808642361912, 'HRI', 'URI')</t>
@@ -103,7 +166,16 @@
     <t>(-0.06427591992427106, 'GIC', 'IGC')</t>
   </si>
   <si>
-    <t>Chemicals</t>
+    <t>Gas Utilities(13)</t>
+  </si>
+  <si>
+    <t>(0.7084146686824703, 'ATO', 'SWX')</t>
+  </si>
+  <si>
+    <t>(-0.1082765238135015, 'NFG', 'RGCO')</t>
+  </si>
+  <si>
+    <t>Chemicals(55)</t>
   </si>
   <si>
     <t>(0.7563468929285467, 'CE', 'EMN')</t>
@@ -112,7 +184,7 @@
     <t>(-0.20268707348397674, 'ADES', 'NEV')</t>
   </si>
   <si>
-    <t>Insurance</t>
+    <t>Insurance(80)</t>
   </si>
   <si>
     <t>(0.8855548429127549, 'LNC', 'PRU')</t>
@@ -121,7 +193,7 @@
     <t>(-0.18794377816264296, 'UNAM', 'WTM')</t>
   </si>
   <si>
-    <t>Capital Markets</t>
+    <t>Capital Markets(87)</t>
   </si>
   <si>
     <t>(0.867801735645092, 'GS', 'MS')</t>
@@ -130,7 +202,16 @@
     <t>(-0.2835088693097858, 'BK', 'MCA')</t>
   </si>
   <si>
-    <t>Metals &amp; Mining</t>
+    <t>Shell Companies(18)</t>
+  </si>
+  <si>
+    <t>(0.837288871202384, 'CIK', 'NHS')</t>
+  </si>
+  <si>
+    <t>(-0.0967391428152018, 'BHV', 'ISBC')</t>
+  </si>
+  <si>
+    <t>Metals &amp; Mining(95)</t>
   </si>
   <si>
     <t>(0.884734443836443, 'BHP', 'RIO')</t>
@@ -139,7 +220,7 @@
     <t>(-0.13482150226025102, 'GFI', 'SIM')</t>
   </si>
   <si>
-    <t>Construction &amp; Engineering</t>
+    <t>Construction &amp; Engineering(23)</t>
   </si>
   <si>
     <t>(0.8119973382379071, 'LEO', 'VMO')</t>
@@ -148,7 +229,7 @@
     <t>(-0.1299272782381926, 'MYRG', 'VMO')</t>
   </si>
   <si>
-    <t>Automobiles</t>
+    <t>Automobiles(9)</t>
   </si>
   <si>
     <t>(0.7530429906586505, 'THO', 'WGO')</t>
@@ -157,7 +238,43 @@
     <t>(-0.059791530643316326, 'HMC', 'MULN')</t>
   </si>
   <si>
-    <t>Specialty Retail</t>
+    <t>Marine(16)</t>
+  </si>
+  <si>
+    <t>(0.7307717934794619, 'SB', 'SBLK')</t>
+  </si>
+  <si>
+    <t>(-0.1552150942270316, 'GLBS', 'MAV')</t>
+  </si>
+  <si>
+    <t>Household Products(10)</t>
+  </si>
+  <si>
+    <t>(0.9758430561341552, 'CENT', 'CENTA')</t>
+  </si>
+  <si>
+    <t>Water Utilities(13)</t>
+  </si>
+  <si>
+    <t>(0.7542590441534944, 'AWK', 'WTRG')</t>
+  </si>
+  <si>
+    <t>(-0.04084476527343828, 'CDZI', 'PCYO')</t>
+  </si>
+  <si>
+    <t>Internet &amp; Direct Marketing Retail(19)</t>
+  </si>
+  <si>
+    <t>(0.9407083830293044, 'QRTEA', 'QRTEB')</t>
+  </si>
+  <si>
+    <t>Leisure Products(12)</t>
+  </si>
+  <si>
+    <t>(0.642110356920334, 'BC', 'PII')</t>
+  </si>
+  <si>
+    <t>Specialty Retail(63)</t>
   </si>
   <si>
     <t>(0.8105472854076968, 'AZO', 'ORLY')</t>
@@ -166,7 +283,7 @@
     <t>(-0.1396974413613823, 'BBY', 'SBI')</t>
   </si>
   <si>
-    <t>Oil, Gas &amp; Consumable Fuels</t>
+    <t>Oil, Gas &amp; Consumable Fuels(128)</t>
   </si>
   <si>
     <t>(0.9106013366381543, 'DVN', 'MRO')</t>
@@ -175,7 +292,25 @@
     <t>(-0.21890214996055324, 'NCA', 'URG')</t>
   </si>
   <si>
-    <t>Semiconductors &amp; Semiconductor Equipment</t>
+    <t>Consumer Finance(23)</t>
+  </si>
+  <si>
+    <t>(0.8173850228681718, 'COF', 'DFS')</t>
+  </si>
+  <si>
+    <t>(-0.15955696677595288, 'NBH', 'SLMBP')</t>
+  </si>
+  <si>
+    <t>Household Durables(43)</t>
+  </si>
+  <si>
+    <t>(0.8918586680723729, 'DHI', 'LEN')</t>
+  </si>
+  <si>
+    <t>(-0.16940086719660163, 'KOSS', 'WIA')</t>
+  </si>
+  <si>
+    <t>Semiconductors &amp; Semiconductor Equipment(75)</t>
   </si>
   <si>
     <t>(0.8114408925831192, 'ADI', 'TXN')</t>
@@ -184,7 +319,7 @@
     <t>(-0.17801603560411028, 'ACLS', 'MUC')</t>
   </si>
   <si>
-    <t>Aerospace &amp; Defense</t>
+    <t>Aerospace &amp; Defense(43)</t>
   </si>
   <si>
     <t>(0.8219744928965719, 'LMT', 'NOC')</t>
@@ -193,7 +328,7 @@
     <t>(-0.14214991854471348, 'ASTC', 'HEI')</t>
   </si>
   <si>
-    <t>Electrical Equipment</t>
+    <t>Electrical Equipment(31)</t>
   </si>
   <si>
     <t>(0.8048888082084795, 'ETN', 'HUBB')</t>
@@ -202,7 +337,7 @@
     <t>(-0.09017275801105007, 'ESP', 'PLUG')</t>
   </si>
   <si>
-    <t>Textiles, Apparel &amp; Luxury Goods</t>
+    <t>Textiles, Apparel &amp; Luxury Goods(30)</t>
   </si>
   <si>
     <t>(0.715122885890624, 'PVH', 'RL')</t>
@@ -211,7 +346,34 @@
     <t>(-0.12217195516268697, 'COLM', 'EVK')</t>
   </si>
   <si>
-    <t>Commercial Services &amp; Supplies</t>
+    <t>Interactive Media &amp; Services(11)</t>
+  </si>
+  <si>
+    <t>(0.9975308725654178, 'GOOG', 'GOOGL')</t>
+  </si>
+  <si>
+    <t>(-0.06920370535026721, 'DHX', 'LOV')</t>
+  </si>
+  <si>
+    <t>Professional Services(38)</t>
+  </si>
+  <si>
+    <t>(0.7153733175248943, 'KFY', 'RHI')</t>
+  </si>
+  <si>
+    <t>(-0.17350115801112675, 'HQI', 'MHI')</t>
+  </si>
+  <si>
+    <t>Software-Application(13)</t>
+  </si>
+  <si>
+    <t>(0.9400297265480392, 'ETY', 'EXG')</t>
+  </si>
+  <si>
+    <t>(-0.09620594585626585, 'STK', 'TROO')</t>
+  </si>
+  <si>
+    <t>Commercial Services &amp; Supplies(57)</t>
   </si>
   <si>
     <t>(0.8176888952806606, 'RSG', 'WM')</t>
@@ -220,7 +382,16 @@
     <t>(-0.16787974520456328, 'TOMZ', 'VVI')</t>
   </si>
   <si>
-    <t>IT Services</t>
+    <t>Life Sciences Tools &amp; Services(20)</t>
+  </si>
+  <si>
+    <t>(0.719555692261847, 'PKI', 'TMO')</t>
+  </si>
+  <si>
+    <t>(-0.07783792413777668, 'AXDX', 'RGEN')</t>
+  </si>
+  <si>
+    <t>IT Services(58)</t>
   </si>
   <si>
     <t>(0.8858803784155986, 'MA', 'V')</t>
@@ -229,7 +400,7 @@
     <t>(-0.1854744961580359, 'IIM', 'UIS')</t>
   </si>
   <si>
-    <t>Beverages</t>
+    <t>Beverages(22)</t>
   </si>
   <si>
     <t>(0.7454617057952203, 'FMX', 'KOF')</t>
@@ -238,16 +409,13 @@
     <t>(-0.0621981716299691, 'KO', 'REED')</t>
   </si>
   <si>
-    <t>Technology Hardware, Storage &amp; Periph...</t>
-  </si>
-  <si>
-    <t>(0.9398746427877895, 'HPF', 'HPI')</t>
-  </si>
-  <si>
-    <t>(-0.15326342960272465, 'HPF', 'SMED')</t>
-  </si>
-  <si>
-    <t>Health Care Providers &amp; Services</t>
+    <t>Wireless Telecommunication Services(14)</t>
+  </si>
+  <si>
+    <t>(0.9875685480494173, 'AMOV', 'AMX')</t>
+  </si>
+  <si>
+    <t>Health Care Providers &amp; Services(48)</t>
   </si>
   <si>
     <t>(0.8118432344854175, 'DGX', 'LH')</t>
@@ -256,7 +424,16 @@
     <t>(-0.1458622339697846, 'AMEH', 'HUM')</t>
   </si>
   <si>
-    <t>Media</t>
+    <t>Thrifts &amp; Mortgage Finance(52)</t>
+  </si>
+  <si>
+    <t>(0.7688650296074256, 'PFS', 'WSFS')</t>
+  </si>
+  <si>
+    <t>(-0.18766478271233544, 'BYM', 'WAFD')</t>
+  </si>
+  <si>
+    <t>Media(47)</t>
   </si>
   <si>
     <t>(0.9899227337087159, 'LBTYA', 'LBTYK')</t>
@@ -265,7 +442,7 @@
     <t>(-0.28221764908029545, 'DJCO', 'TVE')</t>
   </si>
   <si>
-    <t>Real Estate Management &amp; Development</t>
+    <t>Real Estate Management &amp; Development(28)</t>
   </si>
   <si>
     <t>(0.876530610117323, 'CBRE', 'JLL')</t>
@@ -274,7 +451,16 @@
     <t>(-0.18365658878133506, 'FRPH', 'NMT')</t>
   </si>
   <si>
-    <t>Software</t>
+    <t>Diversified Telecommunication Services(21)</t>
+  </si>
+  <si>
+    <t>(0.7208428836987091, 'BCE', 'TU')</t>
+  </si>
+  <si>
+    <t>(-0.1438431870766541, 'GSAT', 'VZ')</t>
+  </si>
+  <si>
+    <t>Software(70)</t>
   </si>
   <si>
     <t>(0.7221481243370496, 'ADSK', 'PTC')</t>
@@ -283,16 +469,16 @@
     <t>(-0.3010840948427318, 'CDR', 'NLOK')</t>
   </si>
   <si>
-    <t>Electronic Equipment, Instruments &amp; C...</t>
-  </si>
-  <si>
-    <t>(0.7945914805764392, 'ARW', 'AVT')</t>
-  </si>
-  <si>
-    <t>(-0.23341537977905125, 'ELTK', 'TAIT')</t>
-  </si>
-  <si>
-    <t>Communications Equipment</t>
+    <t>Diversified Consumer Services(18)</t>
+  </si>
+  <si>
+    <t>(0.5050019521443372, 'ATGE', 'STRA')</t>
+  </si>
+  <si>
+    <t>(-0.09935156345912377, 'STON', 'WW')</t>
+  </si>
+  <si>
+    <t>Communications Equipment(50)</t>
   </si>
   <si>
     <t>(0.6704047477288283, 'FFIV', 'JNPR')</t>
@@ -301,7 +487,7 @@
     <t>(-0.2721004251301993, 'BOSC', 'NOM')</t>
   </si>
   <si>
-    <t>Entertainment</t>
+    <t>Entertainment(26)</t>
   </si>
   <si>
     <t>(0.9720050055581492, 'NCV', 'NCZ')</t>
@@ -310,7 +496,16 @@
     <t>(-0.1133171536591886, 'GAIA', 'IQI')</t>
   </si>
   <si>
-    <t>Health Care Equipment &amp; Supplies</t>
+    <t>Food &amp; Staples Retailing(15)</t>
+  </si>
+  <si>
+    <t>(0.5393310747466386, 'SPTN', 'WMK')</t>
+  </si>
+  <si>
+    <t>(-0.07177722377446472, 'CBD', 'IMKTA')</t>
+  </si>
+  <si>
+    <t>Health Care Equipment &amp; Supplies(87)</t>
   </si>
   <si>
     <t>(0.6693853184747948, 'SYK', 'ZBH')</t>
@@ -319,7 +514,7 @@
     <t>(-0.245937572403365, 'MMU', 'STXS')</t>
   </si>
   <si>
-    <t>Food Products</t>
+    <t>Food Products(47)</t>
   </si>
   <si>
     <t>(0.8342581510738292, 'SENEA', 'SENEB')</t>
@@ -328,7 +523,16 @@
     <t>(-0.18521000769639406, 'CALM', 'PMF')</t>
   </si>
   <si>
-    <t>Pharmaceuticals</t>
+    <t>Personal Products(19)</t>
+  </si>
+  <si>
+    <t>(0.6046452928882864, 'HLF', 'NUS')</t>
+  </si>
+  <si>
+    <t>(-0.06844820450929734, 'NAII', 'NHTC')</t>
+  </si>
+  <si>
+    <t>Pharmaceuticals(56)</t>
   </si>
   <si>
     <t>(0.7891538123052999, 'AVK', 'EOS')</t>
@@ -337,7 +541,7 @@
     <t>(-0.1997498977480363, 'OPNT', 'SNOA')</t>
   </si>
   <si>
-    <t>Biotechnology</t>
+    <t>Biotechnology(163)</t>
   </si>
   <si>
     <t>(0.9533543806082179, 'ADX', 'GAM')</t>
@@ -706,17 +910,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -739,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.47503733824541922</v>
+        <v>0.50216438590486379</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -753,27 +957,27 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.43906754992020208</v>
+        <v>0.48019718473546619</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.47503733824541922</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4">
-        <v>0.41930181576452408</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -781,447 +985,811 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.40906438469974971</v>
+        <v>0.44818950249391232</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.43962749975644733</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>0.39015300488517601</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0.43906754992020208</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
-        <v>0.37985265800196127</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>0.3520278566310312</v>
+        <v>0.41896630215599262</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9">
-        <v>0.34341287252846148</v>
+        <v>0.41401901142907882</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10">
-        <v>0.32662966159095802</v>
+        <v>0.40906438469974971</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>0.32194156355554981</v>
+        <v>0.3974404211376279</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12">
-        <v>0.31616350049438963</v>
+        <v>0.39015300488517601</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13">
-        <v>0.3149011815135962</v>
+        <v>0.37985265800196127</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14">
-        <v>0.31323349741153023</v>
+        <v>0.35586554840847329</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B15">
-        <v>0.3126581808148024</v>
+        <v>0.35347045796131288</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>0.30416915062710592</v>
+        <v>0.3520278566310312</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17">
-        <v>0.3037477698449117</v>
+        <v>0.3482561685021982</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B18">
-        <v>0.26957910779207989</v>
+        <v>0.34341287252846148</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B19">
-        <v>0.26916308038349568</v>
+        <v>0.34082609753177973</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B20">
-        <v>0.26642122948141927</v>
+        <v>0.32662966159095802</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B21">
-        <v>0.26627489606660443</v>
+        <v>0.32194156355554981</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B22">
-        <v>0.2580903919249159</v>
+        <v>0.31616350049438963</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B23">
-        <v>0.25400151125170112</v>
+        <v>0.31530709946175972</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B24">
-        <v>0.25316950012553369</v>
+        <v>0.3149011815135962</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B25">
-        <v>0.23907213930532359</v>
+        <v>0.31323349741153023</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B26">
-        <v>0.22693820724164279</v>
+        <v>0.3126581808148024</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B27">
-        <v>0.21173460782312309</v>
+        <v>0.31102052019195781</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B28">
-        <v>0.2075758485591509</v>
+        <v>0.3103392647940571</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B29">
-        <v>0.20136805404239999</v>
+        <v>0.30657394559334128</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B30">
-        <v>0.1969074937874504</v>
+        <v>0.30623144845658901</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B31">
-        <v>0.19174614177595661</v>
+        <v>0.30493668812657743</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B32">
-        <v>0.18495520857302561</v>
+        <v>0.30416915062710592</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B33">
-        <v>0.17135637202664691</v>
+        <v>0.3037477698449117</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B34">
-        <v>0.15508368022834521</v>
+        <v>0.28753286726740218</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B35">
-        <v>0.1398704832191926</v>
+        <v>0.27322017796350101</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36">
+        <v>0.26957910779207989</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37">
+        <v>0.26916308038349568</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38">
+        <v>0.26642122948141927</v>
+      </c>
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>105</v>
       </c>
-      <c r="B36">
+      <c r="B39">
+        <v>0.26627489606660443</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40">
+        <v>0.26593638727795321</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41">
+        <v>0.26541669301793702</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42">
+        <v>0.26064467651577722</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43">
+        <v>0.2580903919249159</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44">
+        <v>0.25706112215157789</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45">
+        <v>0.25400151125170112</v>
+      </c>
+      <c r="C45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46">
+        <v>0.25316950012553369</v>
+      </c>
+      <c r="C46" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47">
+        <v>0.24819974536468239</v>
+      </c>
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48">
+        <v>0.22693820724164279</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49">
+        <v>0.21762770442708579</v>
+      </c>
+      <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50">
+        <v>0.21173460782312309</v>
+      </c>
+      <c r="C50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51">
+        <v>0.2075758485591509</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52">
+        <v>0.20642542605153419</v>
+      </c>
+      <c r="C52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53">
+        <v>0.20136805404239999</v>
+      </c>
+      <c r="C53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54">
+        <v>0.19631130460033239</v>
+      </c>
+      <c r="C54" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55">
+        <v>0.19174614177595661</v>
+      </c>
+      <c r="C55" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56">
+        <v>0.18495520857302561</v>
+      </c>
+      <c r="C56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57">
+        <v>0.17671476466803229</v>
+      </c>
+      <c r="C57" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58">
+        <v>0.17135637202664691</v>
+      </c>
+      <c r="C58" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59">
+        <v>0.15508368022834521</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>167</v>
+      </c>
+      <c r="B60">
+        <v>0.14164764180146461</v>
+      </c>
+      <c r="C60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61">
+        <v>0.1398704832191926</v>
+      </c>
+      <c r="C61" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62">
         <v>0.12624262657492269</v>
       </c>
-      <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" t="s">
-        <v>107</v>
+      <c r="C62" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>